<commit_message>
Modified File To Fail Specific Test Case
</commit_message>
<xml_diff>
--- a/Book1.xlsx
+++ b/Book1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\justi\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{BF99BB66-6D22-4D62-8BE2-5A5C5D39D388}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD5F8C25-436D-4F8E-B2C6-431AC1C670BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{DA69B48A-7C3A-45AE-85C8-60851242BCA3}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="9">
   <si>
     <t>Numbers</t>
   </si>
@@ -47,10 +47,22 @@
     <t>Symbol</t>
   </si>
   <si>
+    <t>*</t>
+  </si>
+  <si>
+    <t>#</t>
+  </si>
+  <si>
+    <t>%</t>
+  </si>
+  <si>
+    <t>^</t>
+  </si>
+  <si>
+    <t>+</t>
+  </si>
+  <si>
     <t>c</t>
-  </si>
-  <si>
-    <t>*</t>
   </si>
 </sst>
 </file>
@@ -405,7 +417,7 @@
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -430,10 +442,10 @@
         <v>1234</v>
       </c>
       <c r="B2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" t="s">
         <v>3</v>
-      </c>
-      <c r="C2" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
@@ -441,7 +453,7 @@
         <v>4356</v>
       </c>
       <c r="B3" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="C3" t="s">
         <v>4</v>
@@ -452,10 +464,10 @@
         <v>4321</v>
       </c>
       <c r="B4" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="C4" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
@@ -463,21 +475,21 @@
         <v>2334</v>
       </c>
       <c r="B5" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="C5" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6">
-        <v>2354</v>
+        <v>235</v>
       </c>
       <c r="B6" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="C6" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>